<commit_message>
Fazendo relatorios de comparação da cidade Manaus e São Paulo
</commit_message>
<xml_diff>
--- a/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
+++ b/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>35°</t>
+          <t>34°</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -488,12 +488,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>55%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>60%</t>
+          <t>59%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -604,7 +604,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -631,17 +631,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>25°</t>
+          <t>26°</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -673,12 +673,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>33°</t>
+          <t>35°</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -710,12 +710,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>71%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -747,12 +747,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>35°</t>
+          <t>34°</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -784,7 +784,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -798,43 +798,6 @@
         </is>
       </c>
       <c r="G10" t="inlineStr">
-        <is>
-          <t>0 de 11</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>qui. 03</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>33°</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>25°</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>90%</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Extremo</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
         <is>
           <t>0 de 11</t>
         </is>

</xml_diff>

<commit_message>
Ajeitando o formato dos graficos de comparação
</commit_message>
<xml_diff>
--- a/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
+++ b/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -525,12 +525,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -552,12 +552,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>36°</t>
+          <t>35°</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>35°</t>
+          <t>34°</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -747,12 +747,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">

</xml_diff>

<commit_message>
Adicionando comentarios no código
</commit_message>
<xml_diff>
--- a/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
+++ b/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,27 +473,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ter. 24</t>
+          <t>qua. 25</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>35°</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>25°</t>
+          <t>26°</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>56%</t>
+          <t>61%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>83%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -510,12 +510,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>qua. 25</t>
+          <t>qui. 26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>36°</t>
+          <t>35°</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -525,12 +525,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>58%</t>
+          <t>61%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -547,22 +547,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>qui. 26</t>
+          <t>sex. 27</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>35°</t>
+          <t>34°</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>25°</t>
+          <t>26°</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -584,12 +584,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sex. 27</t>
+          <t>sáb. 28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>35°</t>
+          <t>34°</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,12 +599,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -621,27 +621,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sáb. 28</t>
+          <t>dom. 29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>32°</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -658,12 +658,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dom. 29</t>
+          <t>seg. 30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>33°</t>
+          <t>32°</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -673,12 +673,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -695,12 +695,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>seg. 30</t>
+          <t>ter. 01</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>31°</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -710,12 +710,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -732,12 +732,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ter. 01</t>
+          <t>qua. 02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>32°</t>
+          <t>34°</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -747,12 +747,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>72%</t>
+          <t>68%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -769,12 +769,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>qua. 02</t>
+          <t>qui. 03</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>33°</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -784,20 +784,57 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>71%</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>91%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Extremo</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0 de 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sex. 04</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>33°</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>25°</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>69%</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>90%</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Extremo</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>89%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Extremo</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>0 de 11</t>
         </is>

</xml_diff>

<commit_message>
Mudando os nomes dos titulos dos gráficos
</commit_message>
<xml_diff>
--- a/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
+++ b/bot-coleta-de-dados-climáticos/dados_clima_manaus.xlsx
@@ -483,12 +483,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>61%</t>
+          <t>58%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -520,17 +520,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>61%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -552,22 +552,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>35°</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>64%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -589,22 +589,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>33°</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>26°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>66%</t>
+          <t>67%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -636,12 +636,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -705,17 +705,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>25°</t>
+          <t>24°</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>76%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -737,22 +737,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>34°</t>
+          <t>33°</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>25°</t>
+          <t>24°</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>68%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -774,22 +774,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>33°</t>
+          <t>32°</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>25°</t>
+          <t>24°</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>71%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33°</t>
+          <t>32°</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -821,12 +821,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>69%</t>
+          <t>72%</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>90%</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">

</xml_diff>